<commit_message>
Midiendo tiempos en Radixsort
</commit_message>
<xml_diff>
--- a/RadixSort/graficas.xlsx
+++ b/RadixSort/graficas.xlsx
@@ -334,142 +334,142 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0">
-                  <c:v>7.4123399999999999E-3</c:v>
+                  <c:v>5.1886399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9825199999999999E-3</c:v>
+                  <c:v>3.7061700000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6930599999999999E-3</c:v>
+                  <c:v>3.87722E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.14036E-2</c:v>
+                  <c:v>4.1623100000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.19738E-2</c:v>
+                  <c:v>4.5614399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.36843E-2</c:v>
+                  <c:v>4.9605700000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.42545E-2</c:v>
+                  <c:v>5.2456599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5965E-2</c:v>
+                  <c:v>5.5397500000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.71054E-2</c:v>
+                  <c:v>5.9868900000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.76756E-2</c:v>
+                  <c:v>6.3860200000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.88159E-2</c:v>
+                  <c:v>6.7851400000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.19956299999999999</c:v>
+                  <c:v>7.2983000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.16668E-2</c:v>
+                  <c:v>7.5833899999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.28072E-2</c:v>
+                  <c:v>7.9825199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3947599999999999E-2</c:v>
+                  <c:v>8.3426299999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.50879E-2</c:v>
+                  <c:v>8.6097199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.62283E-2</c:v>
+                  <c:v>0.13741300000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.79388E-2</c:v>
+                  <c:v>9.6360399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.9079199999999999E-2</c:v>
+                  <c:v>9.9781499999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.02195E-2</c:v>
+                  <c:v>0.103773</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.1359900000000003E-2</c:v>
+                  <c:v>0.106624</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.2500300000000003E-2</c:v>
+                  <c:v>0.110045</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.36406E-2</c:v>
+                  <c:v>0.113466</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.5351199999999999E-2</c:v>
+                  <c:v>0.11802700000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.7061700000000003E-2</c:v>
+                  <c:v>0.122589</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.7691299999999997E-2</c:v>
+                  <c:v>0.12772</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.93424E-2</c:v>
+                  <c:v>0.13057099999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.9912599999999999E-2</c:v>
+                  <c:v>0.140264</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.1623100000000003E-2</c:v>
+                  <c:v>0.18987000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.3333700000000003E-2</c:v>
+                  <c:v>0.25715100000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.50442E-2</c:v>
+                  <c:v>0.25544099999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.196712</c:v>
+                  <c:v>0.25373000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.259432</c:v>
+                  <c:v>0.26627400000000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.12772</c:v>
+                  <c:v>0.25601099999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.120878</c:v>
+                  <c:v>0.26114199999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.1886399999999999E-2</c:v>
+                  <c:v>0.338117</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.1886399999999999E-2</c:v>
+                  <c:v>0.30390600000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.5307500000000002E-2</c:v>
+                  <c:v>0.28223900000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.4737300000000003E-2</c:v>
+                  <c:v>0.32386199999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.12486899999999999</c:v>
+                  <c:v>0.336976</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.15451899999999999</c:v>
+                  <c:v>0.29364299999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.147677</c:v>
+                  <c:v>0.30447600000000002</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.14995700000000001</c:v>
+                  <c:v>0.30219499999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.1009300000000002E-2</c:v>
+                  <c:v>0.30219499999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.15794</c:v>
+                  <c:v>0.80737499999999995</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.15794</c:v>
+                  <c:v>0.39627499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2688,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,7 +2717,7 @@
         <v>150</v>
       </c>
       <c r="D4" s="1">
-        <v>7.4123399999999999E-3</v>
+        <v>5.1886399999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2730,7 +2730,7 @@
         <v>180</v>
       </c>
       <c r="D5" s="1">
-        <v>7.9825199999999999E-3</v>
+        <v>3.7061700000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>210</v>
       </c>
       <c r="D6" s="1">
-        <v>9.6930599999999999E-3</v>
+        <v>3.87722E-2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
         <v>240</v>
       </c>
       <c r="D7" s="1">
-        <v>1.14036E-2</v>
+        <v>4.1623100000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2769,7 +2769,7 @@
         <v>270</v>
       </c>
       <c r="D8" s="1">
-        <v>1.19738E-2</v>
+        <v>4.5614399999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>300</v>
       </c>
       <c r="D9" s="1">
-        <v>1.36843E-2</v>
+        <v>4.9605700000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>330</v>
       </c>
       <c r="D10" s="1">
-        <v>1.42545E-2</v>
+        <v>5.2456599999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
         <v>360</v>
       </c>
       <c r="D11" s="1">
-        <v>1.5965E-2</v>
+        <v>5.5397500000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2821,7 +2821,7 @@
         <v>390</v>
       </c>
       <c r="D12" s="1">
-        <v>1.71054E-2</v>
+        <v>5.9868900000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>420</v>
       </c>
       <c r="D13" s="1">
-        <v>1.76756E-2</v>
+        <v>6.3860200000000006E-2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>450</v>
       </c>
       <c r="D14" s="1">
-        <v>1.88159E-2</v>
+        <v>6.7851400000000006E-2</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>480</v>
       </c>
       <c r="D15" s="1">
-        <v>0.19956299999999999</v>
+        <v>7.2983000000000006E-2</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -2873,7 +2873,7 @@
         <v>510</v>
       </c>
       <c r="D16" s="1">
-        <v>2.16668E-2</v>
+        <v>7.5833899999999996E-2</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
         <v>540</v>
       </c>
       <c r="D17" s="1">
-        <v>2.28072E-2</v>
+        <v>7.9825199999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -2899,7 +2899,7 @@
         <v>570</v>
       </c>
       <c r="D18" s="1">
-        <v>2.3947599999999999E-2</v>
+        <v>8.3426299999999995E-2</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -2912,7 +2912,7 @@
         <v>600</v>
       </c>
       <c r="D19" s="1">
-        <v>2.50879E-2</v>
+        <v>8.6097199999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>630</v>
       </c>
       <c r="D20" s="1">
-        <v>2.62283E-2</v>
+        <v>0.13741300000000001</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -2938,7 +2938,7 @@
         <v>660</v>
       </c>
       <c r="D21" s="1">
-        <v>2.79388E-2</v>
+        <v>9.6360399999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -2951,7 +2951,7 @@
         <v>690</v>
       </c>
       <c r="D22" s="1">
-        <v>2.9079199999999999E-2</v>
+        <v>9.9781499999999995E-2</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>720</v>
       </c>
       <c r="D23" s="1">
-        <v>3.02195E-2</v>
+        <v>0.103773</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>750</v>
       </c>
       <c r="D24" s="1">
-        <v>3.1359900000000003E-2</v>
+        <v>0.106624</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
         <v>780</v>
       </c>
       <c r="D25" s="1">
-        <v>3.2500300000000003E-2</v>
+        <v>0.110045</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -3003,7 +3003,7 @@
         <v>810</v>
       </c>
       <c r="D26" s="1">
-        <v>3.36406E-2</v>
+        <v>0.113466</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>840</v>
       </c>
       <c r="D27" s="1">
-        <v>3.5351199999999999E-2</v>
+        <v>0.11802700000000001</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -3029,7 +3029,7 @@
         <v>870</v>
       </c>
       <c r="D28" s="1">
-        <v>3.7061700000000003E-2</v>
+        <v>0.122589</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>900</v>
       </c>
       <c r="D29" s="1">
-        <v>3.7691299999999997E-2</v>
+        <v>0.12772</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -3055,7 +3055,7 @@
         <v>930</v>
       </c>
       <c r="D30" s="1">
-        <v>3.93424E-2</v>
+        <v>0.13057099999999999</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
         <v>960</v>
       </c>
       <c r="D31" s="1">
-        <v>3.9912599999999999E-2</v>
+        <v>0.140264</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>990</v>
       </c>
       <c r="D32" s="1">
-        <v>4.1623100000000003E-2</v>
+        <v>0.18987000000000001</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
         <v>1020</v>
       </c>
       <c r="D33" s="1">
-        <v>4.3333700000000003E-2</v>
+        <v>0.25715100000000002</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
         <v>1050</v>
       </c>
       <c r="D34" s="1">
-        <v>4.50442E-2</v>
+        <v>0.25544099999999997</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>1080</v>
       </c>
       <c r="D35" s="1">
-        <v>0.196712</v>
+        <v>0.25373000000000001</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -3133,7 +3133,7 @@
         <v>1110</v>
       </c>
       <c r="D36" s="1">
-        <v>0.259432</v>
+        <v>0.26627400000000001</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -3146,7 +3146,7 @@
         <v>1140</v>
       </c>
       <c r="D37" s="1">
-        <v>0.12772</v>
+        <v>0.25601099999999999</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
         <v>1170</v>
       </c>
       <c r="D38" s="1">
-        <v>0.120878</v>
+        <v>0.26114199999999999</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>1200</v>
       </c>
       <c r="D39" s="1">
-        <v>5.1886399999999999E-2</v>
+        <v>0.338117</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>1230</v>
       </c>
       <c r="D40" s="1">
-        <v>5.1886399999999999E-2</v>
+        <v>0.30390600000000001</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
         <v>1260</v>
       </c>
       <c r="D41" s="1">
-        <v>5.5307500000000002E-2</v>
+        <v>0.28223900000000002</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -3211,7 +3211,7 @@
         <v>1290</v>
       </c>
       <c r="D42" s="1">
-        <v>5.4737300000000003E-2</v>
+        <v>0.32386199999999998</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>1320</v>
       </c>
       <c r="D43" s="1">
-        <v>0.12486899999999999</v>
+        <v>0.336976</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -3237,7 +3237,7 @@
         <v>1350</v>
       </c>
       <c r="D44" s="1">
-        <v>0.15451899999999999</v>
+        <v>0.29364299999999999</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>1380</v>
       </c>
       <c r="D45" s="1">
-        <v>0.147677</v>
+        <v>0.30447600000000002</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>1410</v>
       </c>
       <c r="D46" s="1">
-        <v>0.14995700000000001</v>
+        <v>0.30219499999999999</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -3276,7 +3276,7 @@
         <v>1440</v>
       </c>
       <c r="D47" s="1">
-        <v>6.1009300000000002E-2</v>
+        <v>0.30219499999999999</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
         <v>1470</v>
       </c>
       <c r="D48" s="1">
-        <v>0.15794</v>
+        <v>0.80737499999999995</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>1500</v>
       </c>
       <c r="D49" s="1">
-        <v>0.15794</v>
+        <v>0.39627499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>